<commit_message>
Added a misspelled word.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E7E641-70A6-4978-81CE-1767B5F728EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EA9668-69D1-41B6-944E-3539028F37CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -50,12 +50,18 @@
   <si>
     <t>lettuces</t>
   </si>
+  <si>
+    <t>Curicullum</t>
+  </si>
+  <si>
+    <t>Curriculum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +86,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,13 +132,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -141,11 +156,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,7 +478,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -601,10 +618,14 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
@@ -966,5 +987,6 @@
     <mergeCell ref="B2:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Practiced Cambridge 14 Test 2.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDCC979-5A17-4154-B36C-B2D9EDE6E7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D30FCE-ECED-41B5-9CFB-D97A33193D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>aesthetic</t>
+  </si>
+  <si>
+    <t>eqipment</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>funiture</t>
+  </si>
+  <si>
+    <t>furniture</t>
   </si>
 </sst>
 </file>
@@ -502,7 +514,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,8 +754,12 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -758,8 +774,12 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>

</xml_diff>

<commit_message>
Practiced Cambridge 14 Test 3.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D30FCE-ECED-41B5-9CFB-D97A33193D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEF3878-A4F5-451B-A74B-91F140F2C9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>furniture</t>
+  </si>
+  <si>
+    <t>Olympic</t>
+  </si>
+  <si>
+    <t>Olympics</t>
+  </si>
+  <si>
+    <t>encourishing</t>
+  </si>
+  <si>
+    <t>encouraging</t>
   </si>
 </sst>
 </file>
@@ -514,7 +526,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,8 +806,12 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -810,8 +826,12 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>

</xml_diff>

<commit_message>
Practiced a Phrasal Verbs lesson and added some misspelled words.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E407F299-C312-49C6-A043-6CF792D1418E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EFB2C6-E399-4C08-8983-59F478A39399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>entrance</t>
+  </si>
+  <si>
+    <t>marrage</t>
+  </si>
+  <si>
+    <t>marriage</t>
+  </si>
+  <si>
+    <t>belive</t>
+  </si>
+  <si>
+    <t>believe</t>
   </si>
 </sst>
 </file>
@@ -564,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE2BE65-1CC2-4D31-AB72-F2E4F74D8764}">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1025,8 +1037,12 @@
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1041,8 +1057,12 @@
       <c r="O23" s="3"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>

</xml_diff>

<commit_message>
Practiced Cambridge 17 Test 2.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EFB2C6-E399-4C08-8983-59F478A39399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1798EE00-D5FF-424B-A17A-398097D1CDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>believe</t>
+  </si>
+  <si>
+    <t>billingual</t>
+  </si>
+  <si>
+    <t>bilingual</t>
   </si>
 </sst>
 </file>
@@ -576,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE2BE65-1CC2-4D31-AB72-F2E4F74D8764}">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1077,8 +1083,12 @@
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>

</xml_diff>

<commit_message>
Added a misspelled vocab.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3014B0-0398-4796-9F91-56600A8CF8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75AE609-9529-4347-B1E6-668336011994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>identify</t>
+  </si>
+  <si>
+    <t>scarf</t>
+  </si>
+  <si>
+    <t>scraf</t>
+  </si>
+  <si>
+    <t>enviroment</t>
+  </si>
+  <si>
+    <t>environment</t>
   </si>
 </sst>
 </file>
@@ -270,7 +282,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -595,7 +609,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -750,8 +764,12 @@
         <v>9</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -770,8 +788,12 @@
         <v>11</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>

</xml_diff>

<commit_message>
Practice Cambridge 9 Test 3.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A388190-4C5E-418C-8C0B-37EEA444C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4851B6BE-6391-42CD-B27E-5BCC4B1F5F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>accidently</t>
+  </si>
+  <si>
+    <t>staticstics</t>
+  </si>
+  <si>
+    <t>statistics</t>
   </si>
 </sst>
 </file>
@@ -645,7 +651,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -992,8 +998,12 @@
         <v>25</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>

</xml_diff>

<commit_message>
Cambridge 13 test 3 Listening Practiced.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D533396-A269-4513-891C-15162172CC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53824485-42BA-4A5F-A1AD-706794F3C410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>seperate</t>
+  </si>
+  <si>
+    <t>permenant</t>
+  </si>
+  <si>
+    <t>permanent</t>
+  </si>
+  <si>
+    <t>indury</t>
+  </si>
+  <si>
+    <t>injury</t>
   </si>
 </sst>
 </file>
@@ -657,7 +669,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1052,8 +1064,12 @@
         <v>28</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1072,8 +1088,12 @@
         <v>31</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>

</xml_diff>

<commit_message>
Practiced IELTS Ready Mock Test 1 Writing.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53824485-42BA-4A5F-A1AD-706794F3C410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E42974B-22E4-4A1C-8240-5835776F28B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -244,6 +244,18 @@
   </si>
   <si>
     <t>injury</t>
+  </si>
+  <si>
+    <t>competative</t>
+  </si>
+  <si>
+    <t>competitive</t>
+  </si>
+  <si>
+    <t>disatisfaction</t>
+  </si>
+  <si>
+    <t>dissatisfaction</t>
   </si>
 </sst>
 </file>
@@ -669,7 +681,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1112,8 +1124,12 @@
         <v>33</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1132,8 +1148,12 @@
         <v>35</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>

</xml_diff>

<commit_message>
Practiced IELTS Ready Mock Test 4 except Writing.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E42974B-22E4-4A1C-8240-5835776F28B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0F5DF1-A6D5-408A-B2BF-92A8D41EAB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -135,9 +135,6 @@
     <t>outnumbered</t>
   </si>
   <si>
-    <t>equipments</t>
-  </si>
-  <si>
     <t>enterance</t>
   </si>
   <si>
@@ -256,6 +253,12 @@
   </si>
   <si>
     <t>dissatisfaction</t>
+  </si>
+  <si>
+    <t>antenna</t>
+  </si>
+  <si>
+    <t>antana</t>
   </si>
 </sst>
 </file>
@@ -681,7 +684,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,10 +792,10 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="3"/>
@@ -813,10 +816,10 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="3"/>
@@ -837,10 +840,10 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
@@ -861,10 +864,10 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -885,10 +888,10 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="3"/>
@@ -909,10 +912,10 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
@@ -933,10 +936,10 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="3"/>
@@ -957,10 +960,10 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="3"/>
@@ -981,10 +984,10 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="3"/>
@@ -1005,10 +1008,10 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="3"/>
@@ -1029,10 +1032,10 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="3"/>
@@ -1053,10 +1056,10 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="3"/>
@@ -1077,10 +1080,10 @@
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="3"/>
@@ -1101,10 +1104,10 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="3"/>
@@ -1125,10 +1128,10 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="3"/>
@@ -1149,7 +1152,7 @@
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>76</v>
@@ -1166,10 +1169,10 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="3"/>
@@ -1186,10 +1189,10 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="3"/>
@@ -1206,10 +1209,10 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
@@ -1226,10 +1229,10 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="3"/>
@@ -1246,10 +1249,10 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="3"/>

</xml_diff>

<commit_message>
Practiced IELTS Ready Mock Test 5.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A530DDCC-A7A1-4786-9B1A-248EA5AD16B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8284F1-B956-428B-AA01-AF94E6B53A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -265,6 +265,24 @@
   </si>
   <si>
     <t>meantime</t>
+  </si>
+  <si>
+    <t>accomodation</t>
+  </si>
+  <si>
+    <t>accommodation</t>
+  </si>
+  <si>
+    <t>enourmous</t>
+  </si>
+  <si>
+    <t>enormous</t>
+  </si>
+  <si>
+    <t>unevitably</t>
+  </si>
+  <si>
+    <t>inevitably</t>
   </si>
 </sst>
 </file>
@@ -689,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE2BE65-1CC2-4D31-AB72-F2E4F74D8764}">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1205,8 +1223,12 @@
         <v>37</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1225,8 +1247,12 @@
         <v>39</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1245,8 +1271,12 @@
         <v>41</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G24" s="4"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>

</xml_diff>

<commit_message>
Added another misspelled word.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB716A7-8B5F-478C-BCE5-CC7941022A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436266B8-F523-43ED-9CFE-F11D6C33EC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t>suicidal</t>
+  </si>
+  <si>
+    <t>secetary</t>
+  </si>
+  <si>
+    <t>secretary</t>
   </si>
 </sst>
 </file>
@@ -744,7 +750,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -998,8 +1004,12 @@
         <v>55</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>

</xml_diff>

<commit_message>
Practice an IELTS Computer Friendly Mock Test.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35622B9-0D05-4B13-858F-9EE2887CE042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706F3346-41DE-4A36-973F-2DD39CBE524A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="142">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -445,6 +445,12 @@
   </si>
   <si>
     <t>activities</t>
+  </si>
+  <si>
+    <t>acessories</t>
+  </si>
+  <si>
+    <t>accessories</t>
   </si>
 </sst>
 </file>
@@ -870,7 +876,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1183,8 +1189,12 @@
         <v>101</v>
       </c>
       <c r="J11" s="4"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="M11" s="4"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>

</xml_diff>

<commit_message>
Practiced Premium Mock Test 3.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD45445-465B-4477-A924-9C1056F99029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E9F8CE-EFCA-4981-BE79-19CB497AE60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -900,7 +900,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Cambridge 16 Test 2 Practiced.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E9F8CE-EFCA-4981-BE79-19CB497AE60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54CD28E-3FA6-4E61-BD91-D97138C8A36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="162">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -475,6 +475,42 @@
   </si>
   <si>
     <t>preferances</t>
+  </si>
+  <si>
+    <t>pleague</t>
+  </si>
+  <si>
+    <t>plague</t>
+  </si>
+  <si>
+    <t>autum</t>
+  </si>
+  <si>
+    <t>autumn</t>
+  </si>
+  <si>
+    <t>Syberia</t>
+  </si>
+  <si>
+    <t>Siberia</t>
+  </si>
+  <si>
+    <t>anticeptive</t>
+  </si>
+  <si>
+    <t>antiseptic</t>
+  </si>
+  <si>
+    <t>nurf</t>
+  </si>
+  <si>
+    <t>nerf</t>
+  </si>
+  <si>
+    <t>obeisity</t>
+  </si>
+  <si>
+    <t>obesity</t>
   </si>
 </sst>
 </file>
@@ -900,7 +936,7 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1373,8 +1409,12 @@
         <v>111</v>
       </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="M16" s="4"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -1401,8 +1441,12 @@
         <v>113</v>
       </c>
       <c r="J17" s="4"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="M17" s="4"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1429,8 +1473,12 @@
         <v>115</v>
       </c>
       <c r="J18" s="4"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="K18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="M18" s="4"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -1457,8 +1505,12 @@
         <v>41</v>
       </c>
       <c r="J19" s="4"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="K19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="M19" s="4"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1485,8 +1537,12 @@
         <v>117</v>
       </c>
       <c r="J20" s="4"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="K20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="M20" s="4"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1513,8 +1569,12 @@
         <v>119</v>
       </c>
       <c r="J21" s="4"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="K21" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>

</xml_diff>

<commit_message>
Nailed my Actual IELTS Test Today.Thus, this commit will be the previous commit to the last one, 'test result commit'. It is kinda sad to say goodbye to this repository. Farewell my friend, we did very well together. Our achievement will come out in flying color in 3 days. Thank u my friend.
</commit_message>
<xml_diff>
--- a/myMisspelledWords.xlsx
+++ b/myMisspelledWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\NZs2024_Return\IELTS\my_IELTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9B4BA2-0311-4C41-84F5-A01FD0BC6A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5481F25A-5AA2-4965-99E1-E8185858293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{883ACD4D-8627-4E1A-8D32-737874AC0ED2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="168">
   <si>
     <t>My Misspelled Words</t>
   </si>
@@ -517,6 +517,18 @@
   </si>
   <si>
     <t>consumable</t>
+  </si>
+  <si>
+    <t>increasement</t>
+  </si>
+  <si>
+    <t>increase</t>
+  </si>
+  <si>
+    <t>calory</t>
+  </si>
+  <si>
+    <t>calorie</t>
   </si>
 </sst>
 </file>
@@ -939,14 +951,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE2BE65-1CC2-4D31-AB72-F2E4F74D8764}">
-  <dimension ref="B2:O33"/>
+  <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="16.08984375" customWidth="1"/>
     <col min="2" max="2" width="14.54296875" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" customWidth="1"/>
     <col min="4" max="4" width="4.81640625" customWidth="1"/>
@@ -958,11 +971,12 @@
     <col min="10" max="10" width="4.7265625" customWidth="1"/>
     <col min="11" max="11" width="15.36328125" customWidth="1"/>
     <col min="12" max="12" width="14.1796875" customWidth="1"/>
-    <col min="13" max="13" width="4.81640625" customWidth="1"/>
+    <col min="13" max="13" width="14.6328125" customWidth="1"/>
     <col min="14" max="14" width="13.54296875" customWidth="1"/>
     <col min="15" max="15" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -977,9 +991,6 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="6"/>
@@ -993,9 +1004,6 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
@@ -1031,15 +1039,6 @@
       <c r="L4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
@@ -1069,7 +1068,6 @@
       <c r="L5" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="M5" s="4"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
@@ -1101,7 +1099,6 @@
       <c r="L6" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="M6" s="4"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
@@ -1133,7 +1130,6 @@
       <c r="L7" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="M7" s="4"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
@@ -1165,7 +1161,6 @@
       <c r="L8" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="M8" s="4"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
@@ -1197,7 +1192,6 @@
       <c r="L9" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="M9" s="4"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
@@ -1229,7 +1223,6 @@
       <c r="L10" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="M10" s="4"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
@@ -1261,7 +1254,6 @@
       <c r="L11" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="M11" s="4"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
@@ -1293,7 +1285,6 @@
       <c r="L12" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="M12" s="4"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
@@ -1325,7 +1316,6 @@
       <c r="L13" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="M13" s="4"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
@@ -1357,7 +1347,6 @@
       <c r="L14" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="M14" s="4"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
@@ -1389,7 +1378,6 @@
       <c r="L15" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M15" s="4"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
@@ -1421,7 +1409,6 @@
       <c r="L16" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="M16" s="4"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
@@ -1453,7 +1440,6 @@
       <c r="L17" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="M17" s="4"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
@@ -1485,7 +1471,6 @@
       <c r="L18" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="M18" s="4"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
     </row>
@@ -1517,7 +1502,6 @@
       <c r="L19" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="M19" s="4"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
     </row>
@@ -1549,7 +1533,6 @@
       <c r="L20" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="M20" s="4"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
     </row>
@@ -1581,7 +1564,6 @@
       <c r="L21" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="M21" s="4"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
@@ -1613,7 +1595,6 @@
       <c r="L22" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="M22" s="4"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
@@ -1645,7 +1626,6 @@
       <c r="L23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="M23" s="4"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
@@ -1671,9 +1651,12 @@
         <v>125</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="4"/>
+      <c r="K24" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
@@ -1699,9 +1682,12 @@
         <v>127</v>
       </c>
       <c r="J25" s="4"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="4"/>
+      <c r="K25" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
@@ -1717,7 +1703,6 @@
       <c r="J26" s="4"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="4"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
@@ -1725,46 +1710,39 @@
       <c r="D27" s="4"/>
       <c r="G27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="M27" s="4"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D28" s="4"/>
       <c r="G28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="M28" s="4"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D29" s="4"/>
       <c r="G29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="M29" s="4"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D30" s="4"/>
       <c r="G30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="M30" s="4"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D31" s="4"/>
       <c r="G31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="M31" s="4"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D32" s="4"/>
       <c r="G32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="M33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="B2:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>